<commit_message>
Add FovTrial for Fluorescence visualization Trial: All fluo will overlap as 1 single cell FovTrial: Cell within same FOV will show as stack view
</commit_message>
<xml_diff>
--- a/cook/high_freq_imaging/status_report.xlsx
+++ b/cook/high_freq_imaging/status_report.xlsx
@@ -155,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +172,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF1A4E86"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF008000"/>
       <name val="Calibri"/>
@@ -179,6 +188,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -221,14 +231,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,8 +540,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="26" width="10.7109375" customWidth="1"/>
+    <col min="1" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -578,7 +589,7 @@
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -590,28 +601,28 @@
       <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="F2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -619,7 +630,7 @@
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -631,28 +642,28 @@
       <c r="E3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="3" t="s">
+      <c r="F3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -660,7 +671,7 @@
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -672,28 +683,28 @@
       <c r="E4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="F4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -701,7 +712,7 @@
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -713,28 +724,28 @@
       <c r="E5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="3" t="s">
+      <c r="F5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -742,7 +753,7 @@
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -754,28 +765,28 @@
       <c r="E6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M6" s="3" t="s">
+      <c r="F6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -783,7 +794,7 @@
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -795,28 +806,28 @@
       <c r="E7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="3" t="s">
+      <c r="F7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -824,7 +835,7 @@
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -836,28 +847,28 @@
       <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="3" t="s">
+      <c r="F8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -865,7 +876,7 @@
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -877,28 +888,28 @@
       <c r="E9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M9" s="3" t="s">
+      <c r="F9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -906,7 +917,7 @@
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -918,28 +929,28 @@
       <c r="E10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M10" s="3" t="s">
+      <c r="F10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -947,7 +958,7 @@
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -959,28 +970,28 @@
       <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="3" t="s">
+      <c r="F11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -988,7 +999,7 @@
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1000,28 +1011,28 @@
       <c r="E12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" s="3" t="s">
+      <c r="F12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1029,7 +1040,7 @@
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1041,28 +1052,28 @@
       <c r="E13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M13" s="3" t="s">
+      <c r="F13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M13" s="4" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>